<commit_message>
Feat: implement component Table in readEXCEL
</commit_message>
<xml_diff>
--- a/src/assets/PlantillaInscripcion.xlsx
+++ b/src/assets/PlantillaInscripcion.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adamj\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adamj\Desktop\Projects\Ohh Sansi Project\Frontend\Ohh-Sansi-Frontend\src\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEED8D1D-98FC-488B-BF37-B55FFEBA39DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2516C598-4C1A-45EE-BB9D-72F9F6BD79D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{6C6FE6F8-25BE-4660-81DF-109DD3D1CFA4}"/>
+    <workbookView xWindow="1920" yWindow="1920" windowWidth="13536" windowHeight="5868" xr2:uid="{6C6FE6F8-25BE-4660-81DF-109DD3D1CFA4}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -47,9 +47,6 @@
     <t>NumeroDocumento</t>
   </si>
   <si>
-    <t>Colegio</t>
-  </si>
-  <si>
     <t>Area</t>
   </si>
   <si>
@@ -57,6 +54,9 @@
   </si>
   <si>
     <t>Tutor</t>
+  </si>
+  <si>
+    <t>Institucion</t>
   </si>
 </sst>
 </file>
@@ -118,7 +118,7 @@
     <tableColumn id="1" xr3:uid="{C3E9712C-32D4-4ED6-8534-CE50A8EC3EB8}" name="Nombres"/>
     <tableColumn id="2" xr3:uid="{4C01AEB4-5145-45EA-B2A2-CEBC2DF8F9D0}" name="Apellidos"/>
     <tableColumn id="3" xr3:uid="{41FC75C7-AFE9-45A2-9B0A-E81E8381A2E1}" name="NumeroDocumento"/>
-    <tableColumn id="4" xr3:uid="{9FCBB442-970C-448B-88A4-B0B665610926}" name="Colegio"/>
+    <tableColumn id="4" xr3:uid="{9FCBB442-970C-448B-88A4-B0B665610926}" name="Institucion"/>
     <tableColumn id="5" xr3:uid="{0C4EDB37-A8A6-4FDA-A433-5DC1E31752F5}" name="Area"/>
     <tableColumn id="6" xr3:uid="{971ED9F4-23C3-4EC1-92F0-C7FB9BB5926F}" name="Correo"/>
     <tableColumn id="7" xr3:uid="{9C4FCBE3-162C-4D0B-9AAB-B68B556B1D91}" name="Tutor"/>
@@ -447,7 +447,7 @@
   <dimension ref="A1:G1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -468,16 +468,16 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>5</v>
-      </c>
-      <c r="G1" t="s">
-        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>